<commit_message>
Updating Lecture 26 Handout, Slides, and Spreadsheet.  Also, updating the schedule and minor updated to lab 2, 3, & 4.
</commit_message>
<xml_diff>
--- a/lecture/lecture26.xlsx
+++ b/lecture/lecture26.xlsx
@@ -12402,11 +12402,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="55929088"/>
-        <c:axId val="75465856"/>
+        <c:axId val="96089984"/>
+        <c:axId val="96091520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55929088"/>
+        <c:axId val="96089984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12416,12 +12416,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75465856"/>
+        <c:crossAx val="96091520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75465856"/>
+        <c:axId val="96091520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12432,7 +12432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55929088"/>
+        <c:crossAx val="96089984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12464,7 +12464,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>51</xdr:col>
+      <xdr:col>52</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -12776,10 +12776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2002"/>
+  <dimension ref="A1:R2002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12793,7 +12793,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -12814,11 +12814,12 @@
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="5"/>
       <c r="Q1" s="8"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="8"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -12842,11 +12843,12 @@
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="5"/>
       <c r="Q2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="8"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -12868,13 +12870,13 @@
       <c r="K3" s="8">
         <v>-1.815341082704568</v>
       </c>
-      <c r="M3" s="8"/>
       <c r="N3" s="8"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="5"/>
       <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="8"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
         <v>7</v>
@@ -12892,11 +12894,12 @@
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="5"/>
       <c r="Q4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="8"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -12906,11 +12909,12 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="5"/>
       <c r="Q5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R5" s="8"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -12929,8 +12933,9 @@
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="8"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -12956,8 +12961,9 @@
       <c r="L7" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -12991,15 +12997,16 @@
         <f ca="1">MATCH(K8,INDIRECT(F8):INDIRECT(F9),0)</f>
         <v>25</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="M8" s="8"/>
+      <c r="O8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <f>6.28/(B1*B3)</f>
         <v>47.97566604562094</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f>A8+$B$1</f>
         <v>2.0833333333333333E-5</v>
@@ -13034,15 +13041,16 @@
         <f ca="1">MATCH(K9,INDIRECT(F8):INDIRECT(F9),0)</f>
         <v>1</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="M9" s="8"/>
+      <c r="O9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O9" s="1">
-        <f ca="1">MOD(360*(L8-I8)/O8,360)</f>
+      <c r="P9" s="1">
+        <f ca="1">MOD(360*(L8-I8)/P8,360)</f>
         <v>90.045649306713798</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" ref="A10:A30" si="1">A9+$B$1</f>
         <v>4.1666666666666665E-5</v>
@@ -13055,15 +13063,15 @@
         <f t="shared" ref="C10:C73" si="2">$H$4*B10+$H$3*B9+$H$2*B8-$K$3*C9-$K$2*C8</f>
         <v>2.0358823652887499E-3</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="1">
+      <c r="P10" s="1">
         <f ca="1">20*LOG10(K8/H8)</f>
         <v>-3.0102999334496054</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>6.2500000000000001E-5</v>
@@ -13077,7 +13085,7 @@
         <v>7.7327511161165959E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>8.3333333333333331E-5</v>
@@ -13091,7 +13099,7 @@
         <v>1.8314656235735118E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>1.0416666666666666E-4</v>
@@ -13105,7 +13113,7 @@
         <v>3.4620138796457152E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>1.25E-4</v>
@@ -13119,7 +13127,7 @@
         <v>5.7122935319322735E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>1.4583333333333335E-4</v>
@@ -13133,7 +13141,7 @@
         <v>8.5957180870545685E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>1.6666666666666669E-4</v>
@@ -40835,7 +40843,7 @@
         <v>0.70710678118836412</v>
       </c>
       <c r="C1994" s="1">
-        <f t="shared" ref="C1994:C2057" si="96">$H$4*B1994+$H$3*B1993+$H$2*B1992-$K$3*C1993-$K$2*C1992</f>
+        <f t="shared" ref="C1994:C2002" si="96">$H$4*B1994+$H$3*B1993+$H$2*B1992-$K$3*C1993-$K$2*C1992</f>
         <v>0.49999999999886874</v>
       </c>
     </row>

</xml_diff>